<commit_message>
Initial commit with most recent survey data export & cleaning up script names.
</commit_message>
<xml_diff>
--- a/Excel/CollectorList.xlsx
+++ b/Excel/CollectorList.xlsx
@@ -91,10 +91,10 @@
     <t>Email Invitation 19</t>
   </si>
   <si>
+    <t>Email Invitation 21</t>
+  </si>
+  <si>
     <t>Email Invitation 20</t>
-  </si>
-  <si>
-    <t>Email Invitation 21</t>
   </si>
   <si>
     <t>Email Invitation 22</t>
@@ -735,7 +735,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="n">
-        <v>172055522</v>
+        <v>172055613</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
@@ -746,7 +746,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="n">
-        <v>172055613</v>
+        <v>172055522</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>

</xml_diff>